<commit_message>
#2 Update MiniExcel Test to read sheet
</commit_message>
<xml_diff>
--- a/test/Cactus.MiniExcelNUnitTest/TestExcelFile.xlsx
+++ b/test/Cactus.MiniExcelNUnitTest/TestExcelFile.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.MiniExcelNUnitTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9277552-12C8-4C34-BAC8-BF6CD449041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A27EFF-A97C-4290-A458-33E4C11CDD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{0BED3855-2AA3-43F5-AEF6-4AF9E20534DC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0BED3855-2AA3-43F5-AEF6-4AF9E20534DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateCount="250" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
@@ -36,12 +37,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Test </t>
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>Another</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -415,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D70C0E-043D-4029-A314-1118ED6D850F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -440,4 +453,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE97F681-FB8A-485C-8AC6-2440CA3A95B5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>